<commit_message>
begining of work for version 2
</commit_message>
<xml_diff>
--- a/meta/indicator.xlsx
+++ b/meta/indicator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeder\Dropbox\VID\wicdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Private\gabel\GitHub\wcde\meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="indicator" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="136">
   <si>
     <t>name</t>
   </si>
@@ -384,9 +384,6 @@
   </si>
   <si>
     <t>past</t>
-  </si>
-  <si>
-    <t>edu2</t>
   </si>
   <si>
     <t>The percentage of the population who are alive for a five-year period in five-year age groups. Available in all scenarios and at all geographical scales. It is expressed as a percentage.</t>
@@ -470,7 +467,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -974,48 +971,48 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1317,13 +1314,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S32"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -1333,18 +1330,17 @@
     <col min="6" max="6" width="5" customWidth="1"/>
     <col min="7" max="7" width="4" customWidth="1"/>
     <col min="8" max="8" width="4.42578125" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" customWidth="1"/>
-    <col min="12" max="12" width="4.7109375" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.140625" customWidth="1"/>
-    <col min="15" max="16" width="9.140625" customWidth="1"/>
-    <col min="17" max="17" width="255.5703125" customWidth="1"/>
-    <col min="18" max="18" width="175.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" customWidth="1"/>
+    <col min="16" max="16" width="255.5703125" customWidth="1"/>
+    <col min="17" max="17" width="175.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -1370,40 +1366,37 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>110</v>
+        <v>61</v>
       </c>
       <c r="J1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K1" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
       <c r="L1" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="M1" t="s">
-        <v>135</v>
+        <v>64</v>
       </c>
       <c r="N1" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="O1" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="P1" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="Q1" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="R1" t="s">
-        <v>63</v>
-      </c>
-      <c r="S1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1435,32 +1428,29 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2">
         <v>1</v>
       </c>
-      <c r="M2">
-        <v>1</v>
+      <c r="M2" t="s">
+        <v>66</v>
       </c>
       <c r="N2" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="P2" t="s">
-        <v>69</v>
+        <v>114</v>
       </c>
       <c r="Q2" t="s">
-        <v>115</v>
-      </c>
-      <c r="R2" t="s">
         <v>10</v>
       </c>
-      <c r="S2"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R2"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -1492,31 +1482,28 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
         <v>1</v>
       </c>
-      <c r="M3">
-        <v>1</v>
+      <c r="M3" t="s">
+        <v>66</v>
       </c>
       <c r="N3" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="P3" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="Q3" t="s">
-        <v>116</v>
-      </c>
-      <c r="R3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>76</v>
       </c>
@@ -1548,30 +1535,27 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
+        <v>66</v>
       </c>
       <c r="N4" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="P4" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>117</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="Q4"/>
       <c r="R4"/>
-      <c r="S4"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1603,31 +1587,28 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
+        <v>66</v>
       </c>
       <c r="N5" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="P5" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="Q5" t="s">
-        <v>102</v>
-      </c>
-      <c r="R5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -1659,31 +1640,28 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
+        <v>66</v>
       </c>
       <c r="N6" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="P6" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="Q6" t="s">
-        <v>103</v>
-      </c>
-      <c r="R6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -1712,7 +1690,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -1720,26 +1698,23 @@
       <c r="L7">
         <v>1</v>
       </c>
-      <c r="M7">
-        <v>1</v>
+      <c r="M7" t="s">
+        <v>65</v>
       </c>
       <c r="N7" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="O7" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="P7" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="Q7" t="s">
-        <v>118</v>
-      </c>
-      <c r="R7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>84</v>
       </c>
@@ -1768,7 +1743,7 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -1776,26 +1751,23 @@
       <c r="L8">
         <v>1</v>
       </c>
-      <c r="M8">
-        <v>1</v>
+      <c r="M8" t="s">
+        <v>65</v>
       </c>
       <c r="N8" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="O8" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="P8" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="Q8" t="s">
-        <v>119</v>
-      </c>
-      <c r="R8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1827,31 +1799,28 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9">
         <v>1</v>
       </c>
-      <c r="M9">
-        <v>1</v>
+      <c r="M9" t="s">
+        <v>66</v>
       </c>
       <c r="N9" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="P9" t="s">
-        <v>69</v>
+        <v>119</v>
       </c>
       <c r="Q9" t="s">
-        <v>120</v>
-      </c>
-      <c r="R9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1877,7 +1846,7 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -1888,29 +1857,26 @@
       <c r="L10">
         <v>1</v>
       </c>
-      <c r="M10">
-        <v>1</v>
+      <c r="M10" t="s">
+        <v>65</v>
       </c>
       <c r="N10" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="O10" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="P10" t="s">
-        <v>74</v>
+        <v>120</v>
       </c>
       <c r="Q10" t="s">
-        <v>121</v>
+        <v>10</v>
       </c>
       <c r="R10" t="s">
-        <v>10</v>
-      </c>
-      <c r="S10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1942,31 +1908,28 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11">
         <v>1</v>
       </c>
-      <c r="M11">
-        <v>1</v>
+      <c r="M11" t="s">
+        <v>66</v>
       </c>
       <c r="N11" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="P11" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
       <c r="Q11" t="s">
-        <v>122</v>
-      </c>
-      <c r="R11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1998,31 +1961,28 @@
         <v>0</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
-      <c r="M12">
-        <v>1</v>
+      <c r="M12" t="s">
+        <v>66</v>
       </c>
       <c r="N12" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="P12" t="s">
-        <v>69</v>
+        <v>122</v>
       </c>
       <c r="Q12" t="s">
-        <v>123</v>
-      </c>
-      <c r="R12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -2057,28 +2017,25 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="M13" t="s">
+        <v>66</v>
       </c>
       <c r="N13" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="P13" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="Q13" t="s">
-        <v>124</v>
-      </c>
-      <c r="R13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -2104,40 +2061,37 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <v>1</v>
       </c>
       <c r="K14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="M14" t="s">
+        <v>67</v>
       </c>
       <c r="N14" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
       <c r="O14" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="P14" t="s">
-        <v>75</v>
+        <v>124</v>
       </c>
       <c r="Q14" t="s">
-        <v>125</v>
+        <v>29</v>
       </c>
       <c r="R14" t="s">
-        <v>29</v>
-      </c>
-      <c r="S14" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -2163,40 +2117,37 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15">
         <v>1</v>
       </c>
       <c r="K15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="M15" t="s">
+        <v>67</v>
       </c>
       <c r="N15" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
       <c r="O15" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="P15" t="s">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="Q15" t="s">
-        <v>126</v>
+        <v>29</v>
       </c>
       <c r="R15" t="s">
-        <v>29</v>
-      </c>
-      <c r="S15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -2222,40 +2173,37 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16">
         <v>1</v>
       </c>
       <c r="K16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="M16" t="s">
+        <v>67</v>
       </c>
       <c r="N16" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
       <c r="O16" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="P16" t="s">
-        <v>75</v>
+        <v>126</v>
       </c>
       <c r="Q16" t="s">
-        <v>127</v>
+        <v>33</v>
       </c>
       <c r="R16" t="s">
-        <v>33</v>
-      </c>
-      <c r="S16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -2287,33 +2235,30 @@
         <v>0</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17">
-        <v>1</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="M17" t="s">
+        <v>66</v>
       </c>
       <c r="N17" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="P17" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q17" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" t="s">
         <v>113</v>
-      </c>
-      <c r="B18" t="s">
-        <v>114</v>
       </c>
       <c r="C18" t="s">
         <v>95</v>
@@ -2340,28 +2285,25 @@
         <v>0</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="M18" t="s">
+        <v>66</v>
       </c>
       <c r="N18" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="P18" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q18" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -2393,28 +2335,25 @@
         <v>0</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19">
-        <v>1</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="M19" t="s">
+        <v>66</v>
       </c>
       <c r="N19" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="P19" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q19" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -2446,28 +2385,25 @@
         <v>0</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20">
-        <v>1</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="M20" t="s">
+        <v>66</v>
       </c>
       <c r="N20" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="P20" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q20" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -2493,34 +2429,31 @@
         <v>1</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21">
         <v>0</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21">
-        <v>1</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="M21" t="s">
+        <v>66</v>
       </c>
       <c r="N21" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="P21" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q21" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -2546,34 +2479,31 @@
         <v>1</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22">
         <v>0</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22">
-        <v>1</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="M22" t="s">
+        <v>66</v>
       </c>
       <c r="N22" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="P22" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q22" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -2602,7 +2532,7 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -2610,26 +2540,23 @@
       <c r="L23">
         <v>1</v>
       </c>
-      <c r="M23">
-        <v>1</v>
+      <c r="M23" t="s">
+        <v>65</v>
       </c>
       <c r="N23" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="O23" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="P23" t="s">
-        <v>71</v>
+        <v>127</v>
       </c>
       <c r="Q23" t="s">
-        <v>128</v>
-      </c>
-      <c r="R23" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -2655,38 +2582,35 @@
         <v>1</v>
       </c>
       <c r="I24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="M24" t="s">
+        <v>65</v>
       </c>
       <c r="N24" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="O24" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="P24" t="s">
-        <v>71</v>
+        <v>128</v>
       </c>
       <c r="Q24" t="s">
-        <v>129</v>
-      </c>
-      <c r="R24" t="s">
         <v>10</v>
       </c>
-      <c r="S24"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R24"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -2715,7 +2639,7 @@
         <v>0</v>
       </c>
       <c r="J25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25">
         <v>1</v>
@@ -2723,26 +2647,23 @@
       <c r="L25">
         <v>1</v>
       </c>
-      <c r="M25">
-        <v>1</v>
+      <c r="M25" t="s">
+        <v>65</v>
       </c>
       <c r="N25" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="O25" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="P25" t="s">
-        <v>71</v>
+        <v>135</v>
       </c>
       <c r="Q25" t="s">
-        <v>136</v>
-      </c>
-      <c r="R25" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -2771,7 +2692,7 @@
         <v>0</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26">
         <v>1</v>
@@ -2779,26 +2700,23 @@
       <c r="L26">
         <v>1</v>
       </c>
-      <c r="M26">
-        <v>1</v>
+      <c r="M26" t="s">
+        <v>65</v>
       </c>
       <c r="N26" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="O26" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="P26" t="s">
-        <v>71</v>
+        <v>129</v>
       </c>
       <c r="Q26" t="s">
-        <v>130</v>
-      </c>
-      <c r="R26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>50</v>
       </c>
@@ -2823,38 +2741,35 @@
       <c r="H27" s="2">
         <v>0</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="2">
         <v>0</v>
       </c>
       <c r="J27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L27" s="2">
-        <v>0</v>
-      </c>
-      <c r="M27" s="2">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>71</v>
+        <v>130</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="R27" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -2883,7 +2798,7 @@
         <v>0</v>
       </c>
       <c r="J28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28">
         <v>1</v>
@@ -2891,26 +2806,23 @@
       <c r="L28">
         <v>1</v>
       </c>
-      <c r="M28">
-        <v>1</v>
+      <c r="M28" t="s">
+        <v>65</v>
       </c>
       <c r="N28" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="O28" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="P28" t="s">
-        <v>72</v>
+        <v>131</v>
       </c>
       <c r="Q28" t="s">
-        <v>132</v>
-      </c>
-      <c r="R28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -2939,7 +2851,7 @@
         <v>0</v>
       </c>
       <c r="J29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29">
         <v>1</v>
@@ -2947,26 +2859,23 @@
       <c r="L29">
         <v>1</v>
       </c>
-      <c r="M29">
-        <v>1</v>
+      <c r="M29" t="s">
+        <v>65</v>
       </c>
       <c r="N29" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="O29" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="P29" t="s">
-        <v>72</v>
+        <v>132</v>
       </c>
       <c r="Q29" t="s">
-        <v>133</v>
-      </c>
-      <c r="R29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -2995,34 +2904,31 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L30">
-        <v>0</v>
-      </c>
-      <c r="M30">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="M30" t="s">
+        <v>65</v>
       </c>
       <c r="N30" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="O30" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="P30" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="Q30" t="s">
-        <v>111</v>
-      </c>
-      <c r="R30" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>98</v>
       </c>
@@ -3051,35 +2957,32 @@
         <v>0</v>
       </c>
       <c r="J31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L31">
-        <v>0</v>
-      </c>
-      <c r="M31">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="M31" t="s">
+        <v>65</v>
       </c>
       <c r="N31" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="O31" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="P31" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="Q31" t="s">
-        <v>112</v>
-      </c>
-      <c r="R31" t="s">
         <v>10</v>
       </c>
-      <c r="S31"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R31"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>99</v>
       </c>
@@ -3108,7 +3011,7 @@
         <v>0</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K32">
         <v>1</v>
@@ -3116,22 +3019,19 @@
       <c r="L32">
         <v>1</v>
       </c>
-      <c r="M32">
-        <v>1</v>
+      <c r="M32" t="s">
+        <v>65</v>
       </c>
       <c r="N32" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="O32" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="P32" t="s">
-        <v>73</v>
+        <v>133</v>
       </c>
       <c r="Q32" t="s">
-        <v>134</v>
-      </c>
-      <c r="R32" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>